<commit_message>
Fix ratio for 1FPB
</commit_message>
<xml_diff>
--- a/data_staged/C2223.xlsx
+++ b/data_staged/C2223.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sdelquin/code/iespuertodelacruz/analitica/data_staged/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0BE0E87-DCC2-2041-B793-A9E7E80CAB96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7356A07-EC18-AA45-B4D8-7A34E5347B81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="E1" sheetId="1" r:id="rId1"/>
@@ -535,7 +535,7 @@
   <dimension ref="A1:H1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -988,7 +988,7 @@
         <v>18</v>
       </c>
       <c r="H18">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>